<commit_message>
H fill actual effort
</commit_message>
<xml_diff>
--- a/Project estimation.xlsx
+++ b/Project estimation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="135">
   <si>
     <t>STT</t>
   </si>
@@ -422,6 +422,9 @@
   </si>
   <si>
     <t>Test tài khoản cá nhân</t>
+  </si>
+  <si>
+    <t>Thống kê effort từng thành viên</t>
   </si>
 </sst>
 </file>
@@ -442,21 +445,25 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -467,12 +474,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -754,7 +763,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -971,6 +980,46 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -986,12 +1035,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1003,39 +1046,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4371,13 +4381,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC1013"/>
+  <dimension ref="A1:AC1014"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -4390,26 +4400,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="15">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="104"/>
-      <c r="I1" s="104"/>
-      <c r="J1" s="104"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:29" ht="15">
-      <c r="A2" s="105"/>
-      <c r="B2" s="105"/>
-      <c r="C2" s="106"/>
+      <c r="A2" s="106"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="107"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5"/>
@@ -4533,7 +4543,7 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:29" ht="15" hidden="1">
+    <row r="8" spans="1:29" ht="15">
       <c r="A8" s="53" t="s">
         <v>18</v>
       </c>
@@ -4546,7 +4556,7 @@
       <c r="E8" s="53"/>
       <c r="F8" s="53">
         <f>SUM(F9:F16)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G8" s="55">
         <v>44284</v>
@@ -4576,9 +4586,9 @@
       <c r="AB8" s="21"/>
       <c r="AC8" s="21"/>
     </row>
-    <row r="9" spans="1:29" ht="15" hidden="1">
+    <row r="9" spans="1:29" ht="15">
       <c r="A9" s="56"/>
-      <c r="B9" s="107" t="s">
+      <c r="B9" s="97" t="s">
         <v>87</v>
       </c>
       <c r="C9" s="57" t="s">
@@ -4598,9 +4608,9 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:29" ht="15" hidden="1">
+    <row r="10" spans="1:29" ht="15">
       <c r="A10" s="58"/>
-      <c r="B10" s="108"/>
+      <c r="B10" s="98"/>
       <c r="C10" s="57" t="s">
         <v>26</v>
       </c>
@@ -4610,7 +4620,9 @@
       <c r="E10" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="F10" s="58"/>
+      <c r="F10" s="58">
+        <v>3</v>
+      </c>
       <c r="G10" s="59"/>
       <c r="H10" s="60"/>
       <c r="I10" s="4"/>
@@ -4618,9 +4630,9 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:29" ht="15" hidden="1">
+    <row r="11" spans="1:29" ht="15">
       <c r="A11" s="58"/>
-      <c r="B11" s="108"/>
+      <c r="B11" s="98"/>
       <c r="C11" s="57" t="s">
         <v>20</v>
       </c>
@@ -4638,9 +4650,9 @@
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:29" ht="15" hidden="1">
+    <row r="12" spans="1:29" ht="15">
       <c r="A12" s="58"/>
-      <c r="B12" s="109"/>
+      <c r="B12" s="99"/>
       <c r="C12" s="57" t="s">
         <v>21</v>
       </c>
@@ -4660,7 +4672,7 @@
     </row>
     <row r="13" spans="1:29" ht="15">
       <c r="A13" s="58"/>
-      <c r="B13" s="110" t="s">
+      <c r="B13" s="101" t="s">
         <v>88</v>
       </c>
       <c r="C13" s="57" t="s">
@@ -4680,9 +4692,9 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:29" ht="15" hidden="1">
+    <row r="14" spans="1:29" ht="15">
       <c r="A14" s="58"/>
-      <c r="B14" s="111"/>
+      <c r="B14" s="102"/>
       <c r="C14" s="57" t="s">
         <v>19</v>
       </c>
@@ -4700,9 +4712,9 @@
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:29" ht="15" hidden="1">
+    <row r="15" spans="1:29" ht="15">
       <c r="A15" s="58"/>
-      <c r="B15" s="111"/>
+      <c r="B15" s="102"/>
       <c r="C15" s="57" t="s">
         <v>89</v>
       </c>
@@ -4720,9 +4732,9 @@
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:29" ht="15" hidden="1">
+    <row r="16" spans="1:29" ht="15">
       <c r="A16" s="58"/>
-      <c r="B16" s="112"/>
+      <c r="B16" s="103"/>
       <c r="C16" s="57" t="s">
         <v>25</v>
       </c>
@@ -4732,7 +4744,9 @@
       <c r="E16" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="F16" s="58"/>
+      <c r="F16" s="58">
+        <v>3</v>
+      </c>
       <c r="G16" s="59"/>
       <c r="H16" s="60"/>
       <c r="I16" s="4"/>
@@ -4740,7 +4754,7 @@
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:29" ht="15" hidden="1">
+    <row r="17" spans="1:29" ht="15">
       <c r="A17" s="53" t="s">
         <v>27</v>
       </c>
@@ -4753,7 +4767,7 @@
       <c r="E17" s="53"/>
       <c r="F17" s="53">
         <f>SUM(F18:F25)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G17" s="55">
         <v>44291</v>
@@ -4783,9 +4797,9 @@
       <c r="AB17" s="21"/>
       <c r="AC17" s="21"/>
     </row>
-    <row r="18" spans="1:29" ht="15" hidden="1">
+    <row r="18" spans="1:29" ht="15">
       <c r="A18" s="58"/>
-      <c r="B18" s="110" t="s">
+      <c r="B18" s="101" t="s">
         <v>96</v>
       </c>
       <c r="C18" s="57" t="s">
@@ -4797,7 +4811,9 @@
       <c r="E18" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="F18" s="58"/>
+      <c r="F18" s="58">
+        <v>5</v>
+      </c>
       <c r="G18" s="62"/>
       <c r="H18" s="62"/>
       <c r="I18" s="4"/>
@@ -4807,7 +4823,7 @@
     </row>
     <row r="19" spans="1:29" ht="15">
       <c r="A19" s="58"/>
-      <c r="B19" s="112"/>
+      <c r="B19" s="103"/>
       <c r="C19" s="57" t="s">
         <v>98</v>
       </c>
@@ -4825,9 +4841,9 @@
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:29" ht="15" hidden="1">
+    <row r="20" spans="1:29" ht="15">
       <c r="A20" s="56"/>
-      <c r="B20" s="107" t="s">
+      <c r="B20" s="97" t="s">
         <v>97</v>
       </c>
       <c r="C20" s="57" t="s">
@@ -4847,9 +4863,9 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:29" ht="15" hidden="1">
+    <row r="21" spans="1:29" ht="15">
       <c r="A21" s="58"/>
-      <c r="B21" s="108"/>
+      <c r="B21" s="98"/>
       <c r="C21" s="57" t="s">
         <v>29</v>
       </c>
@@ -4867,9 +4883,9 @@
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:29" ht="15" hidden="1">
+    <row r="22" spans="1:29" ht="15">
       <c r="A22" s="58"/>
-      <c r="B22" s="108"/>
+      <c r="B22" s="98"/>
       <c r="C22" s="63" t="s">
         <v>30</v>
       </c>
@@ -4887,9 +4903,9 @@
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
     </row>
-    <row r="23" spans="1:29" s="46" customFormat="1" ht="15" hidden="1">
+    <row r="23" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A23" s="58"/>
-      <c r="B23" s="108"/>
+      <c r="B23" s="98"/>
       <c r="C23" s="63" t="s">
         <v>99</v>
       </c>
@@ -4899,7 +4915,9 @@
       <c r="E23" s="65" t="s">
         <v>91</v>
       </c>
-      <c r="F23" s="64"/>
+      <c r="F23" s="64">
+        <v>3</v>
+      </c>
       <c r="G23" s="62"/>
       <c r="H23" s="62"/>
       <c r="I23" s="5"/>
@@ -4907,9 +4925,9 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:29" s="46" customFormat="1" ht="15" hidden="1">
+    <row r="24" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A24" s="58"/>
-      <c r="B24" s="108"/>
+      <c r="B24" s="98"/>
       <c r="C24" s="63" t="s">
         <v>100</v>
       </c>
@@ -4927,9 +4945,9 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:29" s="46" customFormat="1" ht="15" hidden="1">
+    <row r="25" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A25" s="58"/>
-      <c r="B25" s="109"/>
+      <c r="B25" s="99"/>
       <c r="C25" s="63" t="s">
         <v>101</v>
       </c>
@@ -4947,7 +4965,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:29" ht="15" hidden="1">
+    <row r="26" spans="1:29" ht="15">
       <c r="A26" s="53" t="s">
         <v>32</v>
       </c>
@@ -4960,7 +4978,7 @@
       <c r="E26" s="53"/>
       <c r="F26" s="53">
         <f>SUM(F27:F39)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G26" s="55">
         <v>44298</v>
@@ -4990,9 +5008,9 @@
       <c r="AB26" s="21"/>
       <c r="AC26" s="21"/>
     </row>
-    <row r="27" spans="1:29" ht="15" hidden="1">
+    <row r="27" spans="1:29" ht="15">
       <c r="A27" s="58"/>
-      <c r="B27" s="113" t="s">
+      <c r="B27" s="93" t="s">
         <v>102</v>
       </c>
       <c r="C27" s="57" t="s">
@@ -5012,9 +5030,9 @@
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
     </row>
-    <row r="28" spans="1:29" ht="15" hidden="1">
+    <row r="28" spans="1:29" ht="15">
       <c r="A28" s="67"/>
-      <c r="B28" s="114"/>
+      <c r="B28" s="100"/>
       <c r="C28" s="57" t="s">
         <v>105</v>
       </c>
@@ -5024,7 +5042,9 @@
       <c r="E28" s="65" t="s">
         <v>91</v>
       </c>
-      <c r="F28" s="64"/>
+      <c r="F28" s="64">
+        <v>4</v>
+      </c>
       <c r="G28" s="60"/>
       <c r="H28" s="59"/>
       <c r="I28" s="4"/>
@@ -5032,9 +5052,9 @@
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
     </row>
-    <row r="29" spans="1:29" ht="15" hidden="1">
+    <row r="29" spans="1:29" ht="15">
       <c r="A29" s="58"/>
-      <c r="B29" s="114"/>
+      <c r="B29" s="100"/>
       <c r="C29" s="57" t="s">
         <v>106</v>
       </c>
@@ -5052,9 +5072,9 @@
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
     </row>
-    <row r="30" spans="1:29" ht="15" hidden="1">
+    <row r="30" spans="1:29" ht="15">
       <c r="A30" s="68"/>
-      <c r="B30" s="114"/>
+      <c r="B30" s="100"/>
       <c r="C30" s="57" t="s">
         <v>107</v>
       </c>
@@ -5064,7 +5084,9 @@
       <c r="E30" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="F30" s="58"/>
+      <c r="F30" s="58">
+        <v>5</v>
+      </c>
       <c r="G30" s="60"/>
       <c r="H30" s="59"/>
       <c r="I30" s="4"/>
@@ -5072,9 +5094,9 @@
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
     </row>
-    <row r="31" spans="1:29" ht="15" hidden="1">
+    <row r="31" spans="1:29" ht="15">
       <c r="A31" s="68"/>
-      <c r="B31" s="115"/>
+      <c r="B31" s="94"/>
       <c r="C31" s="57" t="s">
         <v>108</v>
       </c>
@@ -5094,7 +5116,7 @@
     </row>
     <row r="32" spans="1:29" ht="15">
       <c r="A32" s="58"/>
-      <c r="B32" s="113" t="s">
+      <c r="B32" s="93" t="s">
         <v>38</v>
       </c>
       <c r="C32" s="57" t="s">
@@ -5114,9 +5136,9 @@
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
     </row>
-    <row r="33" spans="1:29" ht="15" hidden="1">
+    <row r="33" spans="1:29" ht="15">
       <c r="A33" s="58"/>
-      <c r="B33" s="114"/>
+      <c r="B33" s="100"/>
       <c r="C33" s="57" t="s">
         <v>109</v>
       </c>
@@ -5126,7 +5148,9 @@
       <c r="E33" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="F33" s="58"/>
+      <c r="F33" s="58">
+        <v>3</v>
+      </c>
       <c r="G33" s="60"/>
       <c r="H33" s="59"/>
       <c r="I33" s="4"/>
@@ -5134,9 +5158,9 @@
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
     </row>
-    <row r="34" spans="1:29" s="46" customFormat="1" ht="15" hidden="1">
+    <row r="34" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A34" s="58"/>
-      <c r="B34" s="115"/>
+      <c r="B34" s="94"/>
       <c r="C34" s="57" t="s">
         <v>110</v>
       </c>
@@ -5154,9 +5178,9 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="1:29" s="46" customFormat="1" ht="15" hidden="1">
+    <row r="35" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A35" s="58"/>
-      <c r="B35" s="113" t="s">
+      <c r="B35" s="93" t="s">
         <v>103</v>
       </c>
       <c r="C35" s="57" t="s">
@@ -5178,7 +5202,7 @@
     </row>
     <row r="36" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A36" s="58"/>
-      <c r="B36" s="115"/>
+      <c r="B36" s="94"/>
       <c r="C36" s="57" t="s">
         <v>37</v>
       </c>
@@ -5196,9 +5220,9 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="1:29" s="46" customFormat="1" ht="15" hidden="1">
+    <row r="37" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A37" s="58"/>
-      <c r="B37" s="110" t="s">
+      <c r="B37" s="101" t="s">
         <v>104</v>
       </c>
       <c r="C37" s="57" t="s">
@@ -5218,9 +5242,9 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:29" s="46" customFormat="1" ht="15" hidden="1">
+    <row r="38" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A38" s="58"/>
-      <c r="B38" s="111"/>
+      <c r="B38" s="102"/>
       <c r="C38" s="57" t="s">
         <v>112</v>
       </c>
@@ -5238,9 +5262,9 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="1:29" s="46" customFormat="1" ht="15" hidden="1">
+    <row r="39" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A39" s="58"/>
-      <c r="B39" s="112"/>
+      <c r="B39" s="103"/>
       <c r="C39" s="57" t="s">
         <v>36</v>
       </c>
@@ -5258,7 +5282,7 @@
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:29" ht="19.5" hidden="1" customHeight="1">
+    <row r="40" spans="1:29" ht="19.5" customHeight="1">
       <c r="A40" s="53" t="s">
         <v>39</v>
       </c>
@@ -5271,7 +5295,7 @@
       <c r="E40" s="53"/>
       <c r="F40" s="53">
         <f>SUM(F41:F48)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G40" s="55">
         <v>44305</v>
@@ -5301,9 +5325,9 @@
       <c r="AB40" s="21"/>
       <c r="AC40" s="21"/>
     </row>
-    <row r="41" spans="1:29" ht="17.25" hidden="1" customHeight="1">
+    <row r="41" spans="1:29" ht="17.25" customHeight="1">
       <c r="A41" s="58"/>
-      <c r="B41" s="113" t="s">
+      <c r="B41" s="93" t="s">
         <v>113</v>
       </c>
       <c r="C41" s="57" t="s">
@@ -5323,9 +5347,9 @@
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
     </row>
-    <row r="42" spans="1:29" ht="15" hidden="1">
+    <row r="42" spans="1:29" ht="15">
       <c r="A42" s="67"/>
-      <c r="B42" s="115"/>
+      <c r="B42" s="94"/>
       <c r="C42" s="57" t="s">
         <v>116</v>
       </c>
@@ -5335,7 +5359,9 @@
       <c r="E42" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="F42" s="58"/>
+      <c r="F42" s="58">
+        <v>2</v>
+      </c>
       <c r="G42" s="62"/>
       <c r="H42" s="62"/>
       <c r="I42" s="4"/>
@@ -5343,9 +5369,9 @@
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
     </row>
-    <row r="43" spans="1:29" ht="15" hidden="1">
+    <row r="43" spans="1:29" ht="15">
       <c r="A43" s="58"/>
-      <c r="B43" s="113" t="s">
+      <c r="B43" s="93" t="s">
         <v>114</v>
       </c>
       <c r="C43" s="57" t="s">
@@ -5357,7 +5383,9 @@
       <c r="E43" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="F43" s="58"/>
+      <c r="F43" s="58">
+        <v>5</v>
+      </c>
       <c r="G43" s="62"/>
       <c r="H43" s="62"/>
       <c r="I43" s="4"/>
@@ -5367,7 +5395,7 @@
     </row>
     <row r="44" spans="1:29" ht="15">
       <c r="A44" s="68"/>
-      <c r="B44" s="115"/>
+      <c r="B44" s="94"/>
       <c r="C44" s="57" t="s">
         <v>117</v>
       </c>
@@ -5385,9 +5413,9 @@
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
     </row>
-    <row r="45" spans="1:29" ht="15" hidden="1">
+    <row r="45" spans="1:29" ht="15">
       <c r="A45" s="68"/>
-      <c r="B45" s="92" t="s">
+      <c r="B45" s="108" t="s">
         <v>115</v>
       </c>
       <c r="C45" s="57" t="s">
@@ -5409,7 +5437,7 @@
     </row>
     <row r="46" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A46" s="68"/>
-      <c r="B46" s="93"/>
+      <c r="B46" s="109"/>
       <c r="C46" s="57" t="s">
         <v>118</v>
       </c>
@@ -5427,9 +5455,9 @@
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
     </row>
-    <row r="47" spans="1:29" s="46" customFormat="1" ht="15" hidden="1">
+    <row r="47" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A47" s="68"/>
-      <c r="B47" s="93"/>
+      <c r="B47" s="109"/>
       <c r="C47" s="57" t="s">
         <v>119</v>
       </c>
@@ -5447,9 +5475,9 @@
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="1:29" s="46" customFormat="1" ht="15" hidden="1">
+    <row r="48" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A48" s="68"/>
-      <c r="B48" s="94"/>
+      <c r="B48" s="110"/>
       <c r="C48" s="57" t="s">
         <v>120</v>
       </c>
@@ -5467,7 +5495,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
     </row>
-    <row r="49" spans="1:29" ht="15" hidden="1">
+    <row r="49" spans="1:29" ht="15">
       <c r="A49" s="53" t="s">
         <v>45</v>
       </c>
@@ -5475,12 +5503,12 @@
       <c r="C49" s="54"/>
       <c r="D49" s="53">
         <f>SUM(D50:D58)</f>
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E49" s="53"/>
       <c r="F49" s="53">
         <f>SUM(F50:F58)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G49" s="55">
         <v>44312</v>
@@ -5510,9 +5538,9 @@
       <c r="AB49" s="21"/>
       <c r="AC49" s="21"/>
     </row>
-    <row r="50" spans="1:29" ht="15" hidden="1">
+    <row r="50" spans="1:29" ht="15">
       <c r="A50" s="58"/>
-      <c r="B50" s="95" t="s">
+      <c r="B50" s="111" t="s">
         <v>121</v>
       </c>
       <c r="C50" s="57" t="s">
@@ -5532,9 +5560,9 @@
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
     </row>
-    <row r="51" spans="1:29" ht="15" hidden="1">
+    <row r="51" spans="1:29" ht="15">
       <c r="A51" s="58"/>
-      <c r="B51" s="96"/>
+      <c r="B51" s="112"/>
       <c r="C51" s="57" t="s">
         <v>125</v>
       </c>
@@ -5544,7 +5572,9 @@
       <c r="E51" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="F51" s="58"/>
+      <c r="F51" s="58">
+        <v>8</v>
+      </c>
       <c r="G51" s="60"/>
       <c r="H51" s="60"/>
       <c r="I51" s="4"/>
@@ -5554,7 +5584,7 @@
     </row>
     <row r="52" spans="1:29" ht="15">
       <c r="A52" s="68"/>
-      <c r="B52" s="97" t="s">
+      <c r="B52" s="95" t="s">
         <v>131</v>
       </c>
       <c r="C52" s="57" t="s">
@@ -5574,9 +5604,9 @@
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
     </row>
-    <row r="53" spans="1:29" s="47" customFormat="1" ht="15" hidden="1">
+    <row r="53" spans="1:29" s="47" customFormat="1" ht="15">
       <c r="A53" s="68"/>
-      <c r="B53" s="98"/>
+      <c r="B53" s="96"/>
       <c r="C53" s="57" t="s">
         <v>133</v>
       </c>
@@ -5586,7 +5616,9 @@
       <c r="E53" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="F53" s="58"/>
+      <c r="F53" s="58">
+        <v>3</v>
+      </c>
       <c r="G53" s="60"/>
       <c r="H53" s="60"/>
       <c r="I53" s="5"/>
@@ -5594,9 +5626,9 @@
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
     </row>
-    <row r="54" spans="1:29" ht="15" hidden="1">
+    <row r="54" spans="1:29" ht="15">
       <c r="A54" s="68"/>
-      <c r="B54" s="97" t="s">
+      <c r="B54" s="95" t="s">
         <v>122</v>
       </c>
       <c r="C54" s="57" t="s">
@@ -5618,7 +5650,7 @@
     </row>
     <row r="55" spans="1:29" ht="15">
       <c r="A55" s="67"/>
-      <c r="B55" s="98"/>
+      <c r="B55" s="96"/>
       <c r="C55" s="69" t="s">
         <v>127</v>
       </c>
@@ -5632,16 +5664,16 @@
       <c r="G55" s="70"/>
       <c r="H55" s="70"/>
     </row>
-    <row r="56" spans="1:29" ht="15" hidden="1">
+    <row r="56" spans="1:29" ht="15">
       <c r="A56" s="67"/>
-      <c r="B56" s="99" t="s">
+      <c r="B56" s="113" t="s">
         <v>123</v>
       </c>
       <c r="C56" s="69" t="s">
         <v>47</v>
       </c>
       <c r="D56" s="71">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E56" s="67" t="s">
         <v>95</v>
@@ -5651,9 +5683,9 @@
       <c r="H56" s="70"/>
       <c r="I56" s="22"/>
     </row>
-    <row r="57" spans="1:29" ht="15" hidden="1">
+    <row r="57" spans="1:29" ht="15">
       <c r="A57" s="67"/>
-      <c r="B57" s="100"/>
+      <c r="B57" s="114"/>
       <c r="C57" s="69" t="s">
         <v>74</v>
       </c>
@@ -5668,9 +5700,9 @@
       <c r="H57" s="70"/>
       <c r="I57" s="22"/>
     </row>
-    <row r="58" spans="1:29" ht="15" hidden="1">
+    <row r="58" spans="1:29" ht="15">
       <c r="A58" s="67"/>
-      <c r="B58" s="101"/>
+      <c r="B58" s="115"/>
       <c r="C58" s="69" t="s">
         <v>128</v>
       </c>
@@ -5685,19 +5717,19 @@
       <c r="H58" s="70"/>
       <c r="I58" s="22"/>
     </row>
-    <row r="59" spans="1:29" ht="15" hidden="1">
-      <c r="A59" s="102" t="s">
+    <row r="59" spans="1:29" ht="15">
+      <c r="A59" s="116" t="s">
         <v>130</v>
       </c>
-      <c r="B59" s="102"/>
-      <c r="C59" s="102"/>
+      <c r="B59" s="116"/>
+      <c r="C59" s="116"/>
       <c r="D59" s="91">
         <f>SUM(D8,D17,D26,D40,D49)</f>
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F59" s="46">
         <f>SUM(F8,F17,F26,F40,F49)</f>
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="H59" s="22"/>
       <c r="I59" s="22"/>
@@ -5707,68 +5739,84 @@
       <c r="H60" s="22"/>
       <c r="I60" s="22"/>
     </row>
-    <row r="61" spans="1:29" ht="15">
-      <c r="C61" s="69" t="s">
-        <v>91</v>
-      </c>
-      <c r="D61" s="71">
-        <v>49</v>
+    <row r="61" spans="1:29" s="92" customFormat="1" ht="15">
+      <c r="C61" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="D61" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" s="52" t="s">
+        <v>54</v>
       </c>
       <c r="H61" s="22"/>
       <c r="I61" s="22"/>
     </row>
     <row r="62" spans="1:29" ht="15">
       <c r="C62" s="69" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D62" s="71">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="E62" s="67">
+        <v>44</v>
       </c>
       <c r="H62" s="22"/>
       <c r="I62" s="22"/>
     </row>
     <row r="63" spans="1:29" ht="15">
       <c r="C63" s="69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D63" s="71">
-        <v>48</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="E63" s="67"/>
       <c r="H63" s="22"/>
       <c r="I63" s="22"/>
     </row>
     <row r="64" spans="1:29" ht="15">
       <c r="C64" s="69" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D64" s="71">
-        <v>53</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E64" s="67"/>
       <c r="H64" s="22"/>
       <c r="I64" s="22"/>
     </row>
     <row r="65" spans="3:9" ht="15">
       <c r="C65" s="69" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D65" s="71">
         <v>54</v>
       </c>
+      <c r="E65" s="67"/>
       <c r="H65" s="22"/>
       <c r="I65" s="22"/>
     </row>
     <row r="66" spans="3:9" ht="15">
       <c r="C66" s="69" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D66" s="71">
-        <v>48</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="E66" s="67"/>
       <c r="H66" s="22"/>
       <c r="I66" s="22"/>
     </row>
     <row r="67" spans="3:9" ht="15">
-      <c r="D67" s="1"/>
+      <c r="C67" s="69" t="s">
+        <v>90</v>
+      </c>
+      <c r="D67" s="71">
+        <v>48</v>
+      </c>
+      <c r="E67" s="67"/>
       <c r="H67" s="22"/>
       <c r="I67" s="22"/>
     </row>
@@ -10502,15 +10550,22 @@
       <c r="H1013" s="22"/>
       <c r="I1013" s="22"/>
     </row>
+    <row r="1014" spans="4:9" ht="15">
+      <c r="D1014" s="1"/>
+      <c r="H1014" s="22"/>
+      <c r="I1014" s="22"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A7:H59">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Trinh"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A7:H59"/>
   <mergeCells count="18">
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B18:B19"/>
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="B43:B44"/>
     <mergeCell ref="B52:B53"/>
@@ -10519,16 +10574,8 @@
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="B37:B39"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B18:B19"/>
     <mergeCell ref="B45:B48"/>
     <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="A59:C59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -10552,20 +10599,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="117" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A2" s="117" t="s">
+      <c r="A2" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="118"/>
+      <c r="B2" s="119"/>
       <c r="C2" s="23"/>
       <c r="D2" s="4"/>
       <c r="E2" s="24" t="s">
@@ -10574,10 +10621,10 @@
       <c r="F2" s="25"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A3" s="117" t="s">
+      <c r="A3" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="118"/>
+      <c r="B3" s="119"/>
       <c r="C3" s="26"/>
       <c r="D3" s="4"/>
       <c r="E3" s="27" t="s">
@@ -10588,10 +10635,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A4" s="117" t="s">
+      <c r="A4" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="118"/>
+      <c r="B4" s="119"/>
       <c r="C4" s="29"/>
       <c r="D4" s="4"/>
       <c r="E4" s="27" t="s">

</xml_diff>

<commit_message>
thuong cap nhat lai
</commit_message>
<xml_diff>
--- a/Project estimation.xlsx
+++ b/Project estimation.xlsx
@@ -986,18 +986,30 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1005,9 +1017,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1019,12 +1028,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1039,18 +1051,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4394,8 +4394,8 @@
   </sheetPr>
   <dimension ref="A1:AC1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -4408,26 +4408,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="15">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:29" ht="15">
-      <c r="A2" s="106"/>
-      <c r="B2" s="106"/>
-      <c r="C2" s="107"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="102"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5"/>
@@ -4596,7 +4596,7 @@
     </row>
     <row r="9" spans="1:29" ht="15">
       <c r="A9" s="56"/>
-      <c r="B9" s="97" t="s">
+      <c r="B9" s="103" t="s">
         <v>87</v>
       </c>
       <c r="C9" s="57" t="s">
@@ -4620,7 +4620,7 @@
     </row>
     <row r="10" spans="1:29" ht="15" hidden="1">
       <c r="A10" s="58"/>
-      <c r="B10" s="98"/>
+      <c r="B10" s="104"/>
       <c r="C10" s="57" t="s">
         <v>26</v>
       </c>
@@ -4642,7 +4642,7 @@
     </row>
     <row r="11" spans="1:29" ht="15" hidden="1">
       <c r="A11" s="58"/>
-      <c r="B11" s="98"/>
+      <c r="B11" s="104"/>
       <c r="C11" s="57" t="s">
         <v>20</v>
       </c>
@@ -4662,7 +4662,7 @@
     </row>
     <row r="12" spans="1:29" ht="15" hidden="1">
       <c r="A12" s="58"/>
-      <c r="B12" s="99"/>
+      <c r="B12" s="105"/>
       <c r="C12" s="57" t="s">
         <v>21</v>
       </c>
@@ -4682,7 +4682,7 @@
     </row>
     <row r="13" spans="1:29" ht="15" hidden="1">
       <c r="A13" s="58"/>
-      <c r="B13" s="101" t="s">
+      <c r="B13" s="106" t="s">
         <v>88</v>
       </c>
       <c r="C13" s="57" t="s">
@@ -4706,7 +4706,7 @@
     </row>
     <row r="14" spans="1:29" ht="15" hidden="1">
       <c r="A14" s="58"/>
-      <c r="B14" s="102"/>
+      <c r="B14" s="107"/>
       <c r="C14" s="57" t="s">
         <v>19</v>
       </c>
@@ -4726,7 +4726,7 @@
     </row>
     <row r="15" spans="1:29" ht="15" hidden="1">
       <c r="A15" s="58"/>
-      <c r="B15" s="102"/>
+      <c r="B15" s="107"/>
       <c r="C15" s="57" t="s">
         <v>89</v>
       </c>
@@ -4748,7 +4748,7 @@
     </row>
     <row r="16" spans="1:29" ht="15" hidden="1">
       <c r="A16" s="58"/>
-      <c r="B16" s="103"/>
+      <c r="B16" s="108"/>
       <c r="C16" s="57" t="s">
         <v>25</v>
       </c>
@@ -4813,7 +4813,7 @@
     </row>
     <row r="18" spans="1:29" ht="15" hidden="1">
       <c r="A18" s="58"/>
-      <c r="B18" s="101" t="s">
+      <c r="B18" s="106" t="s">
         <v>96</v>
       </c>
       <c r="C18" s="57" t="s">
@@ -4837,7 +4837,7 @@
     </row>
     <row r="19" spans="1:29" ht="15" hidden="1">
       <c r="A19" s="58"/>
-      <c r="B19" s="103"/>
+      <c r="B19" s="108"/>
       <c r="C19" s="57" t="s">
         <v>98</v>
       </c>
@@ -4859,7 +4859,7 @@
     </row>
     <row r="20" spans="1:29" ht="15" hidden="1">
       <c r="A20" s="56"/>
-      <c r="B20" s="97" t="s">
+      <c r="B20" s="103" t="s">
         <v>97</v>
       </c>
       <c r="C20" s="57" t="s">
@@ -4883,7 +4883,7 @@
     </row>
     <row r="21" spans="1:29" ht="15" hidden="1">
       <c r="A21" s="58"/>
-      <c r="B21" s="98"/>
+      <c r="B21" s="104"/>
       <c r="C21" s="57" t="s">
         <v>29</v>
       </c>
@@ -4903,7 +4903,7 @@
     </row>
     <row r="22" spans="1:29" ht="15" hidden="1">
       <c r="A22" s="58"/>
-      <c r="B22" s="98"/>
+      <c r="B22" s="104"/>
       <c r="C22" s="63" t="s">
         <v>30</v>
       </c>
@@ -4923,7 +4923,7 @@
     </row>
     <row r="23" spans="1:29" s="46" customFormat="1" ht="15" hidden="1">
       <c r="A23" s="58"/>
-      <c r="B23" s="98"/>
+      <c r="B23" s="104"/>
       <c r="C23" s="63" t="s">
         <v>99</v>
       </c>
@@ -4945,7 +4945,7 @@
     </row>
     <row r="24" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A24" s="58"/>
-      <c r="B24" s="98"/>
+      <c r="B24" s="104"/>
       <c r="C24" s="63" t="s">
         <v>100</v>
       </c>
@@ -4967,7 +4967,7 @@
     </row>
     <row r="25" spans="1:29" s="46" customFormat="1" ht="15" hidden="1">
       <c r="A25" s="58"/>
-      <c r="B25" s="99"/>
+      <c r="B25" s="105"/>
       <c r="C25" s="63" t="s">
         <v>101</v>
       </c>
@@ -5030,7 +5030,7 @@
     </row>
     <row r="27" spans="1:29" ht="15">
       <c r="A27" s="58"/>
-      <c r="B27" s="93" t="s">
+      <c r="B27" s="109" t="s">
         <v>102</v>
       </c>
       <c r="C27" s="57" t="s">
@@ -5054,7 +5054,7 @@
     </row>
     <row r="28" spans="1:29" ht="15" hidden="1">
       <c r="A28" s="67"/>
-      <c r="B28" s="100"/>
+      <c r="B28" s="111"/>
       <c r="C28" s="57" t="s">
         <v>105</v>
       </c>
@@ -5076,7 +5076,7 @@
     </row>
     <row r="29" spans="1:29" ht="15" hidden="1">
       <c r="A29" s="58"/>
-      <c r="B29" s="100"/>
+      <c r="B29" s="111"/>
       <c r="C29" s="57" t="s">
         <v>106</v>
       </c>
@@ -5096,7 +5096,7 @@
     </row>
     <row r="30" spans="1:29" ht="15" hidden="1">
       <c r="A30" s="68"/>
-      <c r="B30" s="100"/>
+      <c r="B30" s="111"/>
       <c r="C30" s="57" t="s">
         <v>107</v>
       </c>
@@ -5118,7 +5118,7 @@
     </row>
     <row r="31" spans="1:29" ht="15" hidden="1">
       <c r="A31" s="68"/>
-      <c r="B31" s="94"/>
+      <c r="B31" s="110"/>
       <c r="C31" s="57" t="s">
         <v>108</v>
       </c>
@@ -5138,7 +5138,7 @@
     </row>
     <row r="32" spans="1:29" ht="15" hidden="1">
       <c r="A32" s="58"/>
-      <c r="B32" s="93" t="s">
+      <c r="B32" s="109" t="s">
         <v>38</v>
       </c>
       <c r="C32" s="57" t="s">
@@ -5162,7 +5162,7 @@
     </row>
     <row r="33" spans="1:29" ht="15" hidden="1">
       <c r="A33" s="58"/>
-      <c r="B33" s="100"/>
+      <c r="B33" s="111"/>
       <c r="C33" s="57" t="s">
         <v>109</v>
       </c>
@@ -5184,7 +5184,7 @@
     </row>
     <row r="34" spans="1:29" s="46" customFormat="1" ht="15" hidden="1">
       <c r="A34" s="58"/>
-      <c r="B34" s="94"/>
+      <c r="B34" s="110"/>
       <c r="C34" s="57" t="s">
         <v>110</v>
       </c>
@@ -5206,7 +5206,7 @@
     </row>
     <row r="35" spans="1:29" s="46" customFormat="1" ht="15" hidden="1">
       <c r="A35" s="58"/>
-      <c r="B35" s="93" t="s">
+      <c r="B35" s="109" t="s">
         <v>103</v>
       </c>
       <c r="C35" s="57" t="s">
@@ -5228,7 +5228,7 @@
     </row>
     <row r="36" spans="1:29" s="46" customFormat="1" ht="15" hidden="1">
       <c r="A36" s="58"/>
-      <c r="B36" s="94"/>
+      <c r="B36" s="110"/>
       <c r="C36" s="57" t="s">
         <v>37</v>
       </c>
@@ -5250,7 +5250,7 @@
     </row>
     <row r="37" spans="1:29" s="46" customFormat="1" ht="15" hidden="1">
       <c r="A37" s="58"/>
-      <c r="B37" s="101" t="s">
+      <c r="B37" s="106" t="s">
         <v>104</v>
       </c>
       <c r="C37" s="57" t="s">
@@ -5274,7 +5274,7 @@
     </row>
     <row r="38" spans="1:29" s="46" customFormat="1" ht="15" hidden="1">
       <c r="A38" s="58"/>
-      <c r="B38" s="102"/>
+      <c r="B38" s="107"/>
       <c r="C38" s="57" t="s">
         <v>112</v>
       </c>
@@ -5294,7 +5294,7 @@
     </row>
     <row r="39" spans="1:29" s="46" customFormat="1" ht="15">
       <c r="A39" s="58"/>
-      <c r="B39" s="103"/>
+      <c r="B39" s="108"/>
       <c r="C39" s="57" t="s">
         <v>36</v>
       </c>
@@ -5359,7 +5359,7 @@
     </row>
     <row r="41" spans="1:29" ht="17.25" customHeight="1">
       <c r="A41" s="58"/>
-      <c r="B41" s="93" t="s">
+      <c r="B41" s="109" t="s">
         <v>113</v>
       </c>
       <c r="C41" s="57" t="s">
@@ -5383,7 +5383,7 @@
     </row>
     <row r="42" spans="1:29" ht="15" hidden="1">
       <c r="A42" s="67"/>
-      <c r="B42" s="94"/>
+      <c r="B42" s="110"/>
       <c r="C42" s="57" t="s">
         <v>116</v>
       </c>
@@ -5405,7 +5405,7 @@
     </row>
     <row r="43" spans="1:29" ht="15" hidden="1">
       <c r="A43" s="58"/>
-      <c r="B43" s="93" t="s">
+      <c r="B43" s="109" t="s">
         <v>114</v>
       </c>
       <c r="C43" s="57" t="s">
@@ -5429,7 +5429,7 @@
     </row>
     <row r="44" spans="1:29" ht="15" hidden="1">
       <c r="A44" s="68"/>
-      <c r="B44" s="94"/>
+      <c r="B44" s="110"/>
       <c r="C44" s="57" t="s">
         <v>117</v>
       </c>
@@ -5451,7 +5451,7 @@
     </row>
     <row r="45" spans="1:29" ht="15" hidden="1">
       <c r="A45" s="68"/>
-      <c r="B45" s="108" t="s">
+      <c r="B45" s="112" t="s">
         <v>115</v>
       </c>
       <c r="C45" s="57" t="s">
@@ -5473,7 +5473,7 @@
     </row>
     <row r="46" spans="1:29" s="46" customFormat="1" ht="15" hidden="1">
       <c r="A46" s="68"/>
-      <c r="B46" s="109"/>
+      <c r="B46" s="113"/>
       <c r="C46" s="57" t="s">
         <v>118</v>
       </c>
@@ -5495,7 +5495,7 @@
     </row>
     <row r="47" spans="1:29" s="46" customFormat="1" ht="15" hidden="1">
       <c r="A47" s="68"/>
-      <c r="B47" s="109"/>
+      <c r="B47" s="113"/>
       <c r="C47" s="57" t="s">
         <v>119</v>
       </c>
@@ -5517,7 +5517,7 @@
     </row>
     <row r="48" spans="1:29" s="46" customFormat="1" ht="15" hidden="1">
       <c r="A48" s="68"/>
-      <c r="B48" s="110"/>
+      <c r="B48" s="114"/>
       <c r="C48" s="57" t="s">
         <v>120</v>
       </c>
@@ -5580,7 +5580,7 @@
     </row>
     <row r="50" spans="1:29" ht="15">
       <c r="A50" s="58"/>
-      <c r="B50" s="111" t="s">
+      <c r="B50" s="115" t="s">
         <v>121</v>
       </c>
       <c r="C50" s="57" t="s">
@@ -5604,7 +5604,7 @@
     </row>
     <row r="51" spans="1:29" ht="15" hidden="1">
       <c r="A51" s="58"/>
-      <c r="B51" s="112"/>
+      <c r="B51" s="116"/>
       <c r="C51" s="57" t="s">
         <v>125</v>
       </c>
@@ -5626,7 +5626,7 @@
     </row>
     <row r="52" spans="1:29" ht="15" hidden="1">
       <c r="A52" s="68"/>
-      <c r="B52" s="95" t="s">
+      <c r="B52" s="93" t="s">
         <v>131</v>
       </c>
       <c r="C52" s="57" t="s">
@@ -5650,7 +5650,7 @@
     </row>
     <row r="53" spans="1:29" s="47" customFormat="1" ht="15" hidden="1">
       <c r="A53" s="68"/>
-      <c r="B53" s="96"/>
+      <c r="B53" s="94"/>
       <c r="C53" s="57" t="s">
         <v>133</v>
       </c>
@@ -5672,7 +5672,7 @@
     </row>
     <row r="54" spans="1:29" ht="15" hidden="1">
       <c r="A54" s="68"/>
-      <c r="B54" s="95" t="s">
+      <c r="B54" s="93" t="s">
         <v>122</v>
       </c>
       <c r="C54" s="57" t="s">
@@ -5694,7 +5694,7 @@
     </row>
     <row r="55" spans="1:29" ht="15" hidden="1">
       <c r="A55" s="67"/>
-      <c r="B55" s="96"/>
+      <c r="B55" s="94"/>
       <c r="C55" s="69" t="s">
         <v>127</v>
       </c>
@@ -5712,7 +5712,7 @@
     </row>
     <row r="56" spans="1:29" ht="15" hidden="1">
       <c r="A56" s="67"/>
-      <c r="B56" s="113" t="s">
+      <c r="B56" s="95" t="s">
         <v>123</v>
       </c>
       <c r="C56" s="69" t="s">
@@ -5733,7 +5733,7 @@
     </row>
     <row r="57" spans="1:29" ht="15" hidden="1">
       <c r="A57" s="67"/>
-      <c r="B57" s="114"/>
+      <c r="B57" s="96"/>
       <c r="C57" s="69" t="s">
         <v>74</v>
       </c>
@@ -5750,7 +5750,7 @@
     </row>
     <row r="58" spans="1:29" ht="15" hidden="1">
       <c r="A58" s="67"/>
-      <c r="B58" s="115"/>
+      <c r="B58" s="97"/>
       <c r="C58" s="69" t="s">
         <v>128</v>
       </c>
@@ -5766,11 +5766,11 @@
       <c r="I58" s="22"/>
     </row>
     <row r="59" spans="1:29" ht="15" hidden="1">
-      <c r="A59" s="116" t="s">
+      <c r="A59" s="98" t="s">
         <v>130</v>
       </c>
-      <c r="B59" s="116"/>
-      <c r="C59" s="116"/>
+      <c r="B59" s="98"/>
+      <c r="C59" s="98"/>
       <c r="D59" s="91">
         <f>SUM(D8,D17,D26,D40,D49)</f>
         <v>305</v>
@@ -5858,10 +5858,7 @@
       <c r="D66" s="71">
         <v>54</v>
       </c>
-      <c r="E66" s="67">
-        <f>F9+F27+F24+F39+F41+F50</f>
-        <v>46</v>
-      </c>
+      <c r="E66" s="67"/>
       <c r="H66" s="22"/>
       <c r="I66" s="22"/>
     </row>
@@ -5872,7 +5869,9 @@
       <c r="D67" s="71">
         <v>48</v>
       </c>
-      <c r="E67" s="67"/>
+      <c r="E67" s="67">
+        <v>46</v>
+      </c>
       <c r="H67" s="22"/>
       <c r="I67" s="22"/>
     </row>
@@ -10620,6 +10619,8 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="18">
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="B50:B51"/>
     <mergeCell ref="B54:B55"/>
     <mergeCell ref="B56:B58"/>
     <mergeCell ref="A59:C59"/>
@@ -10636,8 +10637,6 @@
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="B37:B39"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="B50:B51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -10664,11 +10663,11 @@
       <c r="A1" s="117" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="118" t="s">

</xml_diff>